<commit_message>
Update figures and files
</commit_message>
<xml_diff>
--- a/results/species_ELH.xlsx
+++ b/results/species_ELH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ELH_WestCoast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F8CE4A-7846-4D8A-8EA2-F5B068501473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A884FCAE-D8B9-4642-AF4D-8D06533D03F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,16 +255,16 @@
     <t>16 to 55</t>
   </si>
   <si>
-    <t>15 to 85</t>
-  </si>
-  <si>
     <t>17 to 64</t>
   </si>
   <si>
-    <t>14 to 81</t>
-  </si>
-  <si>
     <t>11 to 78</t>
+  </si>
+  <si>
+    <t>15 to 81</t>
+  </si>
+  <si>
+    <t>21 to 85</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="5">
         <v>35</v>
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5">
         <v>31</v>
@@ -864,7 +864,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D6" s="5">
         <v>35</v>

</xml_diff>